<commit_message>
mise en place des système de validation
ensemble d'erreur permetant le bon fonctionnement de la manipulation des données
</commit_message>
<xml_diff>
--- a/Doc/WIP/Journal-de-Travail_Lordon-Lucas.xlsx
+++ b/Doc/WIP/Journal-de-Travail_Lordon-Lucas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pu61qgw\Documents\GitHub\P_WEB295\Doc\WIP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1BC6D85-837F-46D8-9017-D4A8E4C98336}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9FB7FC1-9FF3-4F3F-931D-9D3460B79C70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="46">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -162,6 +162,21 @@
   </si>
   <si>
     <t>problème avec le curl du post dans insomnia</t>
+  </si>
+  <si>
+    <t>réinstallation puis changement de classe afin de travailler</t>
+  </si>
+  <si>
+    <t>A cause de la convocation, au début nous n'étions pas dans la salle habituelle</t>
+  </si>
+  <si>
+    <t>Faire les automatisation de test insomnia : DELETE/PUT_id/POST/GET_id/Get_all/Error_404</t>
+  </si>
+  <si>
+    <t>Finir la gestion d'erreur sauf pour la route delete</t>
+  </si>
+  <si>
+    <t>faire l'ensemble des validation pour le model t_books</t>
   </si>
 </sst>
 </file>
@@ -617,7 +632,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C26" sqref="C26"/>
+      <selection pane="bottomLeft" activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -682,7 +697,7 @@
       </c>
       <c r="C3" s="22">
         <f>SUM(C5:C521)</f>
-        <v>0.25347222222222227</v>
+        <v>0.33888888888888902</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>13</v>
@@ -1019,42 +1034,71 @@
       <c r="B22" s="9">
         <v>45353</v>
       </c>
-      <c r="C22" s="10"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
+      <c r="C22" s="23">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E22" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="F22" s="11" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="15" t="str">
-        <f>IF(ISBLANK(B23),"",_xlfn.ISOWEEKNUM(Table2[[#This Row],[Jour]]))</f>
-        <v/>
-      </c>
-      <c r="B23" s="9"/>
-      <c r="C23" s="10"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="11"/>
+      <c r="A23" s="15">
+        <v>10</v>
+      </c>
+      <c r="B23" s="9">
+        <v>45353</v>
+      </c>
+      <c r="C23" s="23">
+        <v>2.5694444444444447E-2</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E23" s="11" t="s">
+        <v>43</v>
+      </c>
       <c r="F23" s="11"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="15" t="str">
-        <f>IF(ISBLANK(B24),"",_xlfn.ISOWEEKNUM(Table2[[#This Row],[Jour]]))</f>
-        <v/>
-      </c>
-      <c r="B24" s="9"/>
-      <c r="C24" s="10"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="11"/>
+      <c r="A24" s="15">
+        <v>10</v>
+      </c>
+      <c r="B24" s="9">
+        <v>45353</v>
+      </c>
+      <c r="C24" s="23">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E24" s="11" t="s">
+        <v>44</v>
+      </c>
       <c r="F24" s="11"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="15" t="str">
-        <f>IF(ISBLANK(B25),"",_xlfn.ISOWEEKNUM(Table2[[#This Row],[Jour]]))</f>
-        <v/>
-      </c>
-      <c r="B25" s="9"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="11"/>
-      <c r="E25" s="11"/>
+      <c r="A25" s="15">
+        <v>10</v>
+      </c>
+      <c r="B25" s="9">
+        <v>45353</v>
+      </c>
+      <c r="C25" s="23">
+        <v>3.888888888888889E-2</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E25" s="11" t="s">
+        <v>45</v>
+      </c>
       <c r="F25" s="11"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -6656,26 +6700,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4F20F00DBE2EE49BE9523363A2DF18B" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="83ae57d85107fc73e8c281aedb059e49">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="99ffe1f3-7857-457f-add0-5bdef636f38d" xmlns:ns3="be0d3259-a7ce-4623-88ec-81594dfcbc1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b000e6a26fbebedf4c24f086a5622afe" ns2:_="" ns3:_="">
     <xsd:import namespace="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
@@ -6898,26 +6922,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8EB0028C-89CE-4553-AB94-94DC6E832369}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDECA689-F55E-43C8-8CEF-25DE741768EA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{146BE2DA-6117-4657-9EA0-437EBB1E64B8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6934,4 +6959,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDECA689-F55E-43C8-8CEF-25DE741768EA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8EB0028C-89CE-4553-AB94-94DC6E832369}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Add filter to findAll
</commit_message>
<xml_diff>
--- a/Doc/WIP/Journal-de-Travail_Lordon-Lucas.xlsx
+++ b/Doc/WIP/Journal-de-Travail_Lordon-Lucas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pu61qgw\Documents\GitHub\P_WEB295\Doc\WIP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9FB7FC1-9FF3-4F3F-931D-9D3460B79C70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{025543AB-C617-4735-975D-1D0553180221}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="49">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -177,6 +177,15 @@
   </si>
   <si>
     <t>faire l'ensemble des validation pour le model t_books</t>
+  </si>
+  <si>
+    <t>mise en place du get like (modification du get finAll) pour books</t>
+  </si>
+  <si>
+    <t>discution suite du projet avec sofiene</t>
+  </si>
+  <si>
+    <t>ordre alphabétique + exige Like plus que 1 caractère</t>
   </si>
 </sst>
 </file>
@@ -632,7 +641,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E28" sqref="E28"/>
+      <selection pane="bottomLeft" activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -697,7 +706,7 @@
       </c>
       <c r="C3" s="22">
         <f>SUM(C5:C521)</f>
-        <v>0.33888888888888902</v>
+        <v>0.36319444444444454</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>13</v>
@@ -1102,36 +1111,57 @@
       <c r="F25" s="11"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="15" t="str">
-        <f>IF(ISBLANK(B26),"",_xlfn.ISOWEEKNUM(Table2[[#This Row],[Jour]]))</f>
-        <v/>
-      </c>
-      <c r="B26" s="9"/>
-      <c r="C26" s="10"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="11"/>
+      <c r="A26" s="15">
+        <v>10</v>
+      </c>
+      <c r="B26" s="9">
+        <v>45353</v>
+      </c>
+      <c r="C26" s="23">
+        <v>1.7361111111111112E-2</v>
+      </c>
+      <c r="D26" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E26" s="11" t="s">
+        <v>46</v>
+      </c>
       <c r="F26" s="11"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="15" t="str">
-        <f>IF(ISBLANK(B27),"",_xlfn.ISOWEEKNUM(Table2[[#This Row],[Jour]]))</f>
-        <v/>
-      </c>
-      <c r="B27" s="9"/>
-      <c r="C27" s="10"/>
-      <c r="D27" s="11"/>
-      <c r="E27" s="11"/>
+      <c r="A27" s="15">
+        <v>10</v>
+      </c>
+      <c r="B27" s="9">
+        <v>45353</v>
+      </c>
+      <c r="C27" s="23">
+        <v>3.472222222222222E-3</v>
+      </c>
+      <c r="D27" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E27" s="11" t="s">
+        <v>47</v>
+      </c>
       <c r="F27" s="11"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="15" t="str">
-        <f>IF(ISBLANK(B28),"",_xlfn.ISOWEEKNUM(Table2[[#This Row],[Jour]]))</f>
-        <v/>
-      </c>
-      <c r="B28" s="9"/>
-      <c r="C28" s="10"/>
-      <c r="D28" s="11"/>
-      <c r="E28" s="11"/>
+      <c r="A28" s="15">
+        <v>10</v>
+      </c>
+      <c r="B28" s="9">
+        <v>45353</v>
+      </c>
+      <c r="C28" s="23">
+        <v>3.472222222222222E-3</v>
+      </c>
+      <c r="D28" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E28" s="11" t="s">
+        <v>48</v>
+      </c>
       <c r="F28" s="11"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -6700,6 +6730,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4F20F00DBE2EE49BE9523363A2DF18B" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="83ae57d85107fc73e8c281aedb059e49">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="99ffe1f3-7857-457f-add0-5bdef636f38d" xmlns:ns3="be0d3259-a7ce-4623-88ec-81594dfcbc1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b000e6a26fbebedf4c24f086a5622afe" ns2:_="" ns3:_="">
     <xsd:import namespace="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
@@ -6922,27 +6972,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8EB0028C-89CE-4553-AB94-94DC6E832369}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDECA689-F55E-43C8-8CEF-25DE741768EA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{146BE2DA-6117-4657-9EA0-437EBB1E64B8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6959,23 +7008,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDECA689-F55E-43C8-8CEF-25DE741768EA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8EB0028C-89CE-4553-AB94-94DC6E832369}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Make fk and t_categorie
</commit_message>
<xml_diff>
--- a/Doc/WIP/Journal-de-Travail_Lordon-Lucas.xlsx
+++ b/Doc/WIP/Journal-de-Travail_Lordon-Lucas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pu61qgw\Documents\GitHub\P_WEB295\Doc\WIP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{025543AB-C617-4735-975D-1D0553180221}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07C0E136-F2A9-442D-80C3-5E98A1AAC334}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="52">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -186,6 +186,15 @@
   </si>
   <si>
     <t>ordre alphabétique + exige Like plus que 1 caractère</t>
+  </si>
+  <si>
+    <t>question test</t>
+  </si>
+  <si>
+    <t>discution test + finir la table category (model,mock,routes,sequilize,etc)</t>
+  </si>
+  <si>
+    <t>faire les liason entre t_categorie et t_books</t>
   </si>
 </sst>
 </file>
@@ -641,7 +650,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E30" sqref="E30"/>
+      <selection pane="bottomLeft" activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -706,7 +715,7 @@
       </c>
       <c r="C3" s="22">
         <f>SUM(C5:C521)</f>
-        <v>0.36319444444444454</v>
+        <v>0.45416666666666677</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>13</v>
@@ -1165,36 +1174,60 @@
       <c r="F28" s="11"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="15" t="str">
+      <c r="A29" s="15">
         <f>IF(ISBLANK(B29),"",_xlfn.ISOWEEKNUM(Table2[[#This Row],[Jour]]))</f>
-        <v/>
-      </c>
-      <c r="B29" s="9"/>
-      <c r="C29" s="10"/>
-      <c r="D29" s="11"/>
-      <c r="E29" s="11"/>
+        <v>10</v>
+      </c>
+      <c r="B29" s="9">
+        <v>45355</v>
+      </c>
+      <c r="C29" s="23">
+        <v>7.6388888888888886E-3</v>
+      </c>
+      <c r="D29" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E29" s="11" t="s">
+        <v>49</v>
+      </c>
       <c r="F29" s="11"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="15" t="str">
+      <c r="A30" s="15">
         <f>IF(ISBLANK(B30),"",_xlfn.ISOWEEKNUM(Table2[[#This Row],[Jour]]))</f>
-        <v/>
-      </c>
-      <c r="B30" s="9"/>
-      <c r="C30" s="10"/>
-      <c r="D30" s="11"/>
-      <c r="E30" s="11"/>
+        <v>10</v>
+      </c>
+      <c r="B30" s="9">
+        <v>45355</v>
+      </c>
+      <c r="C30" s="23">
+        <v>2.4999999999999998E-2</v>
+      </c>
+      <c r="D30" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E30" s="11" t="s">
+        <v>50</v>
+      </c>
       <c r="F30" s="11"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="15" t="str">
+      <c r="A31" s="15">
         <f>IF(ISBLANK(B31),"",_xlfn.ISOWEEKNUM(Table2[[#This Row],[Jour]]))</f>
-        <v/>
-      </c>
-      <c r="B31" s="9"/>
-      <c r="C31" s="10"/>
-      <c r="D31" s="11"/>
-      <c r="E31" s="11"/>
+        <v>10</v>
+      </c>
+      <c r="B31" s="9">
+        <v>45355</v>
+      </c>
+      <c r="C31" s="23">
+        <v>5.8333333333333327E-2</v>
+      </c>
+      <c r="D31" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E31" s="11" t="s">
+        <v>51</v>
+      </c>
       <c r="F31" s="11"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -6730,26 +6763,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4F20F00DBE2EE49BE9523363A2DF18B" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="83ae57d85107fc73e8c281aedb059e49">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="99ffe1f3-7857-457f-add0-5bdef636f38d" xmlns:ns3="be0d3259-a7ce-4623-88ec-81594dfcbc1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b000e6a26fbebedf4c24f086a5622afe" ns2:_="" ns3:_="">
     <xsd:import namespace="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
@@ -6972,26 +6985,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8EB0028C-89CE-4553-AB94-94DC6E832369}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDECA689-F55E-43C8-8CEF-25DE741768EA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{146BE2DA-6117-4657-9EA0-437EBB1E64B8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7008,4 +7022,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDECA689-F55E-43C8-8CEF-25DE741768EA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8EB0028C-89CE-4553-AB94-94DC6E832369}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Debug - Still broke
</commit_message>
<xml_diff>
--- a/Doc/WIP/Journal-de-Travail_Lordon-Lucas.xlsx
+++ b/Doc/WIP/Journal-de-Travail_Lordon-Lucas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pu61qgw\Documents\GitHub\P_WEB295\Doc\WIP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07C0E136-F2A9-442D-80C3-5E98A1AAC334}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{591DB095-29E5-40CC-916E-BF8A32AE7E2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="55">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -195,6 +195,15 @@
   </si>
   <si>
     <t>faire les liason entre t_categorie et t_books</t>
+  </si>
+  <si>
+    <t>mettre les codes en commun</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Essayer de régler le problème de FK </t>
+  </si>
+  <si>
+    <t>C'est un enfer et cela ne fonctionne pas…</t>
   </si>
 </sst>
 </file>
@@ -649,7 +658,7 @@
   <dimension ref="A1:N531"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="5" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
@@ -715,7 +724,7 @@
       </c>
       <c r="C3" s="22">
         <f>SUM(C5:C521)</f>
-        <v>0.45416666666666677</v>
+        <v>0.62083333333333346</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>13</v>
@@ -1175,8 +1184,7 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="15">
-        <f>IF(ISBLANK(B29),"",_xlfn.ISOWEEKNUM(Table2[[#This Row],[Jour]]))</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B29" s="9">
         <v>45355</v>
@@ -1194,8 +1202,7 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="15">
-        <f>IF(ISBLANK(B30),"",_xlfn.ISOWEEKNUM(Table2[[#This Row],[Jour]]))</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B30" s="9">
         <v>45355</v>
@@ -1213,8 +1220,7 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="15">
-        <f>IF(ISBLANK(B31),"",_xlfn.ISOWEEKNUM(Table2[[#This Row],[Jour]]))</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B31" s="9">
         <v>45355</v>
@@ -1231,26 +1237,42 @@
       <c r="F31" s="11"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="15" t="str">
-        <f>IF(ISBLANK(B32),"",_xlfn.ISOWEEKNUM(Table2[[#This Row],[Jour]]))</f>
-        <v/>
-      </c>
-      <c r="B32" s="9"/>
-      <c r="C32" s="10"/>
-      <c r="D32" s="11"/>
-      <c r="E32" s="11"/>
+      <c r="A32" s="15">
+        <v>11</v>
+      </c>
+      <c r="B32" s="9">
+        <v>45356</v>
+      </c>
+      <c r="C32" s="23">
+        <v>5.1388888888888894E-2</v>
+      </c>
+      <c r="D32" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E32" s="11" t="s">
+        <v>52</v>
+      </c>
       <c r="F32" s="11"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="15" t="str">
-        <f>IF(ISBLANK(B33),"",_xlfn.ISOWEEKNUM(Table2[[#This Row],[Jour]]))</f>
-        <v/>
-      </c>
-      <c r="B33" s="9"/>
-      <c r="C33" s="10"/>
-      <c r="D33" s="11"/>
-      <c r="E33" s="11"/>
-      <c r="F33" s="11"/>
+      <c r="A33" s="15">
+        <v>11</v>
+      </c>
+      <c r="B33" s="9">
+        <v>45356</v>
+      </c>
+      <c r="C33" s="23">
+        <v>0.11527777777777777</v>
+      </c>
+      <c r="D33" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E33" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="F33" s="11" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="15" t="str">
@@ -6763,6 +6785,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4F20F00DBE2EE49BE9523363A2DF18B" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="83ae57d85107fc73e8c281aedb059e49">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="99ffe1f3-7857-457f-add0-5bdef636f38d" xmlns:ns3="be0d3259-a7ce-4623-88ec-81594dfcbc1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b000e6a26fbebedf4c24f086a5622afe" ns2:_="" ns3:_="">
     <xsd:import namespace="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
@@ -6985,27 +7027,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8EB0028C-89CE-4553-AB94-94DC6E832369}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDECA689-F55E-43C8-8CEF-25DE741768EA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{146BE2DA-6117-4657-9EA0-437EBB1E64B8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7022,23 +7063,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDECA689-F55E-43C8-8CEF-25DE741768EA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8EB0028C-89CE-4553-AB94-94DC6E832369}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>